<commit_message>
Backlog sprint 1 do grupo atualizado
</commit_message>
<xml_diff>
--- a/Docs/ProductBacklog-v2.xlsx
+++ b/Docs/ProductBacklog-v2.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="SprintBacklog" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Escopo</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Tamanho</t>
   </si>
   <si>
-    <t>Os documentos do projeto deverão estar organizados no Github</t>
-  </si>
-  <si>
     <t>As tabelas criadas deverão ser ligadas com a página web para posterior consulta</t>
   </si>
   <si>
@@ -91,6 +88,27 @@
   </si>
   <si>
     <t>Os dados coletados pelo sensor deverão ser enviados para o banco de dados no Azure (Conforme requisito 11)</t>
+  </si>
+  <si>
+    <t>Os documentos do projeto deverão estar organizados no Github e organizar tarefas de cada membro em uma ferramenta de gestão de projetos (Trello)</t>
+  </si>
+  <si>
+    <t>Criar tabelas de banco de dados (Uma tabela para salvar os dados dos usuários informados no requisito 1 e outra para os dados coletados no arduino)</t>
+  </si>
+  <si>
+    <t>Fazer a modelagem conceitual dos dados que irão compor as tabelas</t>
+  </si>
+  <si>
+    <t>Sprint Grupo 1 (Sprint 2)- 16/09 - 23/09</t>
+  </si>
+  <si>
+    <t>O site deverá ter uma tela de cadastro do usuário (Nome, Sobrenome, Email, Telefone, CNPJ, senha)</t>
+  </si>
+  <si>
+    <t>O site deverá ter uma tela de login do usuário (Email, senha)</t>
+  </si>
+  <si>
+    <t>Product Backlog</t>
   </si>
 </sst>
 </file>
@@ -153,7 +171,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +202,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -258,11 +282,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -305,7 +340,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -317,6 +351,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J20"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,13 +680,13 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>1</v>
@@ -629,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -643,7 +711,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="9">
         <v>2</v>
@@ -657,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9">
         <v>3</v>
@@ -671,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="9">
         <v>4</v>
@@ -685,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="9">
         <v>5</v>
@@ -695,13 +763,13 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>6</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="23">
+        <v>10</v>
+      </c>
+      <c r="D7" s="22">
         <v>6</v>
       </c>
       <c r="E7" s="1">
@@ -713,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="9">
         <v>7</v>
@@ -723,13 +791,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="23">
+        <v>19</v>
+      </c>
+      <c r="D9" s="22">
         <v>8</v>
       </c>
       <c r="E9" s="1">
@@ -741,7 +809,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
@@ -755,7 +823,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="9">
         <v>2</v>
@@ -770,7 +838,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="9">
         <v>3</v>
@@ -779,12 +847,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>12</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
@@ -794,39 +862,39 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="34">
         <v>13</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="35">
+        <v>2</v>
+      </c>
+      <c r="E14" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
         <v>14</v>
       </c>
-      <c r="D14" s="9">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="21">
+        <v>15</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="9">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>15</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="D16" s="9">
         <v>4</v>
@@ -839,47 +907,63 @@
       <c r="B17" s="7">
         <v>16</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="14">
+      <c r="C17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="9">
         <v>5</v>
       </c>
-      <c r="E17" s="15">
-        <v>13</v>
+      <c r="E17" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>17</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="C18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14">
         <v>6</v>
       </c>
-      <c r="E18" s="18">
-        <v>8</v>
+      <c r="E18" s="15">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="7">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="21">
-        <f>SUM(E2:E18)</f>
-        <v>110</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="20">
+        <f>SUM(E2:E19)</f>
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B2:E18">
@@ -893,12 +977,306 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="137" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="25">
+        <v>4</v>
+      </c>
+      <c r="D5" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="28">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25">
+        <v>7</v>
+      </c>
+      <c r="D8" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="28">
+        <v>8</v>
+      </c>
+      <c r="D9" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>11</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="25">
+        <v>3</v>
+      </c>
+      <c r="D12" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="35">
+        <v>2</v>
+      </c>
+      <c r="D14" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>14</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="25">
+        <v>3</v>
+      </c>
+      <c r="D15" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="25">
+        <v>4</v>
+      </c>
+      <c r="D16" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="25">
+        <v>5</v>
+      </c>
+      <c r="D17" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>17</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="31">
+        <v>6</v>
+      </c>
+      <c r="D18" s="32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>18</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="25">
+        <v>7</v>
+      </c>
+      <c r="D19" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="20">
+        <f>SUM(D2,D3,D4,D10,D11,D13,D14)</f>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>